<commit_message>
date is working well
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/goldRule.xlsx
+++ b/src/main/resources/rules/goldRule.xlsx
@@ -682,7 +682,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -724,7 +724,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -1002,7 +1002,9 @@
       <c r="E14" s="10">
         <v>500</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="24">
+        <v>41858</v>
+      </c>
       <c r="G14" s="7">
         <v>17</v>
       </c>

</xml_diff>